<commit_message>
update for N0326 release (not send to NECi)
</commit_message>
<xml_diff>
--- a/application/fw_update_win/doc/options.xlsx
+++ b/application/fw_update_win/doc/options.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="38">
   <si>
     <t>Actions</t>
     <phoneticPr fontId="2"/>
@@ -159,6 +159,14 @@
   </si>
   <si>
     <t>check</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>target drive</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/t</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -515,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U34" sqref="U34"/>
+      <selection activeCell="C5" sqref="C5:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -534,10 +542,12 @@
     <col min="9" max="9" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9" style="1"/>
+    <col min="12" max="12" width="9" style="1"/>
+    <col min="13" max="13" width="5.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -572,10 +582,13 @@
         <v>10</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
@@ -609,9 +622,12 @@
       <c r="K2" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M2" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -636,11 +652,11 @@
       <c r="I5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -662,11 +678,11 @@
       <c r="I6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -676,11 +692,11 @@
       <c r="G7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -696,11 +712,11 @@
       <c r="I8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -713,20 +729,17 @@
       <c r="F9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="H9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="N9" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -734,7 +747,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -744,11 +757,11 @@
       <c r="I11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="N11" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -758,11 +771,11 @@
       <c r="K12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="N12" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -770,7 +783,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
update for migration repository to google code
</commit_message>
<xml_diff>
--- a/application/fw_update_win/doc/options.xlsx
+++ b/application/fw_update_win/doc/options.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="38">
   <si>
     <t>Actions</t>
     <phoneticPr fontId="2"/>
@@ -523,10 +523,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -634,9 +635,6 @@
       <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="E5" s="1" t="s">
         <v>13</v>
       </c>
@@ -817,6 +815,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -830,6 +829,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>